<commit_message>
Comments & MU Fields
Added a New MU Field in Import, Export, Add, Update journeys..
Changed Import Format..
Ability to see comments in exported file
</commit_message>
<xml_diff>
--- a/src/import/importFormat.xlsx
+++ b/src/import/importFormat.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubham_gupta5\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\stock\src\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDC4435-01BF-40DC-B1C1-E82AC8915A74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" tabRatio="767"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="16" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Description</t>
   </si>
@@ -113,14 +114,20 @@
   </si>
   <si>
     <t>925  Charms or components</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>MU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$₹-4009]\ #,##0;[Red][$₹-4009]\ #,##0"/>
+    <numFmt numFmtId="164" formatCode="[$₹-4009]\ #,##0;[Red][$₹-4009]\ #,##0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -224,7 +231,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -280,13 +287,13 @@
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 19" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="3"/>
-    <cellStyle name="Normal 5" xfId="4"/>
-    <cellStyle name="Normal 6" xfId="5"/>
-    <cellStyle name="Normal 7" xfId="6"/>
-    <cellStyle name="Normal 8" xfId="7"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 19" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 5" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 6" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 7" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 8" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -701,33 +708,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.47265625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="16.47265625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="17.47265625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.68359375" customWidth="1"/>
-    <col min="5" max="5" width="41" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.15625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.68359375" customWidth="1"/>
-    <col min="8" max="8" width="8.47265625" customWidth="1"/>
-    <col min="9" max="9" width="6.47265625" customWidth="1"/>
-    <col min="10" max="11" width="7.47265625" customWidth="1"/>
-    <col min="12" max="12" width="9.3125" customWidth="1"/>
-    <col min="13" max="13" width="6.83984375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="17.47265625" style="1" customWidth="1"/>
-    <col min="15" max="214" width="10.9453125" customWidth="1"/>
+    <col min="1" max="1" width="7.46875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="12.703125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="10.5859375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.8203125" customWidth="1"/>
+    <col min="5" max="5" width="32.8203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.9375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.52734375" customWidth="1"/>
+    <col min="8" max="8" width="7.29296875" customWidth="1"/>
+    <col min="9" max="9" width="6.46875" customWidth="1"/>
+    <col min="10" max="10" width="7.46875" customWidth="1"/>
+    <col min="11" max="11" width="6.52734375" customWidth="1"/>
+    <col min="12" max="12" width="7.17578125" customWidth="1"/>
+    <col min="13" max="13" width="5.29296875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.8203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.234375" customWidth="1"/>
+    <col min="16" max="16" width="6.234375" customWidth="1"/>
+    <col min="17" max="214" width="10.9375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="6" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
@@ -769,33 +779,39 @@
       </c>
       <c r="N1" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B65397">
     <cfRule type="duplicateValues" dxfId="0" priority="2" stopIfTrue="1"/>
   </conditionalFormatting>
-  <pageMargins left="0.25" right="0.26" top="0.37" bottom="0.32" header="0.3" footer="0.21"/>
-  <pageSetup scale="65" orientation="portrait"/>
+  <pageMargins left="0.1" right="0.1" top="0" bottom="0.75" header="0.25" footer="0.3"/>
+  <pageSetup paperSize="9" scale="65" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="13.47265625" customWidth="1"/>
-    <col min="3" max="256" width="10.9453125" customWidth="1"/>
+    <col min="2" max="2" width="13.46875" customWidth="1"/>
+    <col min="3" max="256" width="10.9375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="20.399999999999999" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" ht="20.7" x14ac:dyDescent="0.7">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
@@ -803,7 +819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
@@ -811,7 +827,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A5" s="13" t="s">
         <v>18</v>
       </c>
@@ -819,7 +835,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A6" s="13" t="s">
         <v>17</v>
       </c>
@@ -827,7 +843,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
@@ -835,7 +851,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A8" s="13" t="s">
         <v>20</v>
       </c>
@@ -843,11 +859,11 @@
         <v>5810</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A9" s="14"/>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
@@ -855,7 +871,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A11" s="15" t="s">
         <v>22</v>
       </c>
@@ -863,7 +879,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A12" s="15" t="s">
         <v>23</v>
       </c>
@@ -871,7 +887,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A13" s="15" t="s">
         <v>24</v>
       </c>
@@ -879,7 +895,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A14" s="15" t="s">
         <v>25</v>
       </c>
@@ -887,11 +903,11 @@
         <v>7510</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A15" s="14"/>
       <c r="B15" s="9"/>
     </row>
-    <row r="16" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A16" s="16" t="s">
         <v>26</v>
       </c>
@@ -899,7 +915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A17" s="16" t="s">
         <v>27</v>
       </c>
@@ -907,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A18" s="16" t="s">
         <v>28</v>
       </c>
@@ -915,7 +931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A19" s="16" t="s">
         <v>29</v>
       </c>
@@ -923,7 +939,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18.3" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.6">
       <c r="A20" s="16" t="s">
         <v>30</v>
       </c>
@@ -933,6 +949,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added CostPrice entry in create, export, import, undo, update flows
</commit_message>
<xml_diff>
--- a/src/import/importFormat.xlsx
+++ b/src/import/importFormat.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\stock\src\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDC4435-01BF-40DC-B1C1-E82AC8915A74}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E4B640-4933-4EDE-B75A-6F62CCBB4EDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="16" r:id="rId1"/>
     <sheet name="Style codes" sheetId="17" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Description</t>
   </si>
@@ -120,6 +120,9 @@
   </si>
   <si>
     <t>MU</t>
+  </si>
+  <si>
+    <t>COST PRICE</t>
   </si>
 </sst>
 </file>
@@ -709,35 +712,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.46875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="12.703125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="10.5859375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.8203125" customWidth="1"/>
-    <col min="5" max="5" width="32.8203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="6.9375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="7.52734375" customWidth="1"/>
-    <col min="8" max="8" width="7.29296875" customWidth="1"/>
-    <col min="9" max="9" width="6.46875" customWidth="1"/>
-    <col min="10" max="10" width="7.46875" customWidth="1"/>
-    <col min="11" max="11" width="6.52734375" customWidth="1"/>
-    <col min="12" max="12" width="7.17578125" customWidth="1"/>
-    <col min="13" max="13" width="5.29296875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="6.8203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.234375" customWidth="1"/>
-    <col min="16" max="16" width="6.234375" customWidth="1"/>
-    <col min="17" max="214" width="10.9375" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="5.77734375" customWidth="1"/>
+    <col min="5" max="5" width="32.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.44140625" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" customWidth="1"/>
+    <col min="11" max="11" width="6.5546875" customWidth="1"/>
+    <col min="12" max="12" width="7.21875" customWidth="1"/>
+    <col min="13" max="13" width="5.33203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="6.77734375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.21875" customWidth="1"/>
+    <col min="16" max="16" width="6.21875" customWidth="1"/>
+    <col min="17" max="214" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="6" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
@@ -785,6 +788,9 @@
       </c>
       <c r="P1" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -804,14 +810,14 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="13.46875" customWidth="1"/>
-    <col min="3" max="256" width="10.9375" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="256" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" ht="20.7" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:2" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
@@ -819,7 +825,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
@@ -827,7 +833,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>18</v>
       </c>
@@ -835,7 +841,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>17</v>
       </c>
@@ -843,7 +849,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>19</v>
       </c>
@@ -851,7 +857,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>20</v>
       </c>
@@ -859,11 +865,11 @@
         <v>5810</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
@@ -871,7 +877,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>22</v>
       </c>
@@ -879,7 +885,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>23</v>
       </c>
@@ -887,7 +893,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>24</v>
       </c>
@@ -895,7 +901,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>25</v>
       </c>
@@ -903,11 +909,11 @@
         <v>7510</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="9"/>
     </row>
-    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>26</v>
       </c>
@@ -915,7 +921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>27</v>
       </c>
@@ -923,7 +929,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>28</v>
       </c>
@@ -931,7 +937,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>29</v>
       </c>
@@ -939,7 +945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Added Three More Columns: Brand, Gold & Silver Price
Export, Import, Update, Edit, Add workflows impacted
</commit_message>
<xml_diff>
--- a/src/import/importFormat.xlsx
+++ b/src/import/importFormat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\stock\src\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41FC3B2-FD0D-48A8-95E0-C4F24AE3E575}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462A79F5-16D9-47B2-872E-3E8198DEDCF5}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Description</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>Vendor PO#</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Gold Price</t>
+  </si>
+  <si>
+    <t>Silver Price</t>
   </si>
 </sst>
 </file>
@@ -141,7 +150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$₹-4009]\ #,##0;[Red][$₹-4009]\ #,##0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +204,12 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -750,11 +765,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U110"/>
+  <dimension ref="A1:W110"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,18 +788,20 @@
     <col min="12" max="12" width="6.5703125" style="20" customWidth="1"/>
     <col min="13" max="13" width="7.28515625" style="20" customWidth="1"/>
     <col min="14" max="14" width="5.28515625" style="20" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="25" customWidth="1"/>
-    <col min="16" max="16" width="8.7109375" style="20" customWidth="1"/>
-    <col min="17" max="17" width="6.7109375" style="20" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" style="20" customWidth="1"/>
-    <col min="19" max="19" width="21.7109375" style="20" customWidth="1"/>
-    <col min="20" max="20" width="9" style="20" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="17" customWidth="1"/>
-    <col min="22" max="217" width="10.85546875" style="17" customWidth="1"/>
-    <col min="218" max="16384" width="8.85546875" style="17"/>
+    <col min="15" max="15" width="6.7109375" style="20" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" style="25" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="20" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" style="20" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="20" customWidth="1"/>
+    <col min="20" max="20" width="21.7109375" style="20" customWidth="1"/>
+    <col min="21" max="21" width="9" style="20" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="17" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" style="17" customWidth="1"/>
+    <col min="24" max="218" width="10.85546875" style="17" customWidth="1"/>
+    <col min="219" max="16384" width="8.85546875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="15" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="15" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
@@ -827,34 +844,46 @@
       <c r="N1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="E2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="U2" s="19"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="23"/>
       <c r="B3" s="18"/>
       <c r="C3" s="22"/>
@@ -869,15 +898,16 @@
       <c r="L3" s="21"/>
       <c r="M3" s="21"/>
       <c r="N3" s="21"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="22"/>
       <c r="Q3" s="21"/>
       <c r="R3" s="21"/>
       <c r="S3" s="21"/>
       <c r="T3" s="21"/>
-      <c r="U3" s="19"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U3" s="21"/>
+      <c r="V3" s="19"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="18"/>
       <c r="C4" s="22"/>
@@ -892,15 +922,16 @@
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="22"/>
       <c r="Q4" s="21"/>
       <c r="R4" s="21"/>
       <c r="S4" s="21"/>
       <c r="T4" s="21"/>
-      <c r="U4" s="19"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U4" s="21"/>
+      <c r="V4" s="19"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="23"/>
       <c r="B5" s="18"/>
       <c r="C5" s="22"/>
@@ -915,15 +946,16 @@
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="22"/>
       <c r="Q5" s="21"/>
       <c r="R5" s="21"/>
       <c r="S5" s="21"/>
       <c r="T5" s="21"/>
-      <c r="U5" s="19"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U5" s="21"/>
+      <c r="V5" s="19"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="23"/>
       <c r="B6" s="18"/>
       <c r="C6" s="22"/>
@@ -938,15 +970,16 @@
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
-      <c r="O6" s="22"/>
-      <c r="P6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="22"/>
       <c r="Q6" s="21"/>
       <c r="R6" s="21"/>
       <c r="S6" s="21"/>
       <c r="T6" s="21"/>
-      <c r="U6" s="19"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U6" s="21"/>
+      <c r="V6" s="19"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="23"/>
       <c r="B7" s="18"/>
       <c r="C7" s="22"/>
@@ -961,15 +994,16 @@
       <c r="L7" s="21"/>
       <c r="M7" s="21"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="22"/>
       <c r="Q7" s="21"/>
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
       <c r="T7" s="21"/>
-      <c r="U7" s="19"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U7" s="21"/>
+      <c r="V7" s="19"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="23"/>
       <c r="B8" s="18"/>
       <c r="C8" s="22"/>
@@ -984,15 +1018,16 @@
       <c r="L8" s="21"/>
       <c r="M8" s="21"/>
       <c r="N8" s="21"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="22"/>
       <c r="Q8" s="21"/>
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
       <c r="T8" s="21"/>
-      <c r="U8" s="19"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U8" s="21"/>
+      <c r="V8" s="19"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="23"/>
       <c r="B9" s="18"/>
       <c r="C9" s="22"/>
@@ -1007,15 +1042,16 @@
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="22"/>
       <c r="Q9" s="21"/>
       <c r="R9" s="21"/>
       <c r="S9" s="21"/>
       <c r="T9" s="21"/>
-      <c r="U9" s="19"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U9" s="21"/>
+      <c r="V9" s="19"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
       <c r="B10" s="18"/>
       <c r="C10" s="22"/>
@@ -1030,15 +1066,16 @@
       <c r="L10" s="21"/>
       <c r="M10" s="21"/>
       <c r="N10" s="21"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="22"/>
       <c r="Q10" s="21"/>
       <c r="R10" s="21"/>
       <c r="S10" s="21"/>
       <c r="T10" s="21"/>
-      <c r="U10" s="19"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U10" s="21"/>
+      <c r="V10" s="19"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
       <c r="B11" s="18"/>
       <c r="C11" s="22"/>
@@ -1053,15 +1090,16 @@
       <c r="L11" s="21"/>
       <c r="M11" s="21"/>
       <c r="N11" s="21"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="22"/>
       <c r="Q11" s="21"/>
       <c r="R11" s="21"/>
       <c r="S11" s="21"/>
       <c r="T11" s="21"/>
-      <c r="U11" s="19"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U11" s="21"/>
+      <c r="V11" s="19"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="18"/>
       <c r="C12" s="22"/>
@@ -1076,15 +1114,16 @@
       <c r="L12" s="21"/>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="22"/>
       <c r="Q12" s="21"/>
       <c r="R12" s="21"/>
       <c r="S12" s="21"/>
       <c r="T12" s="21"/>
-      <c r="U12" s="19"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U12" s="21"/>
+      <c r="V12" s="19"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
       <c r="B13" s="18"/>
       <c r="C13" s="22"/>
@@ -1099,15 +1138,16 @@
       <c r="L13" s="21"/>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="22"/>
       <c r="Q13" s="21"/>
       <c r="R13" s="21"/>
       <c r="S13" s="21"/>
       <c r="T13" s="21"/>
-      <c r="U13" s="19"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U13" s="21"/>
+      <c r="V13" s="19"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
       <c r="B14" s="18"/>
       <c r="C14" s="22"/>
@@ -1122,15 +1162,16 @@
       <c r="L14" s="21"/>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="22"/>
       <c r="Q14" s="21"/>
       <c r="R14" s="21"/>
       <c r="S14" s="21"/>
       <c r="T14" s="21"/>
-      <c r="U14" s="19"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U14" s="21"/>
+      <c r="V14" s="19"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="18"/>
       <c r="C15" s="22"/>
@@ -1145,15 +1186,16 @@
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="22"/>
       <c r="Q15" s="21"/>
       <c r="R15" s="21"/>
       <c r="S15" s="21"/>
       <c r="T15" s="21"/>
-      <c r="U15" s="19"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U15" s="21"/>
+      <c r="V15" s="19"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
       <c r="B16" s="18"/>
       <c r="C16" s="22"/>
@@ -1168,15 +1210,16 @@
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="22"/>
       <c r="Q16" s="21"/>
       <c r="R16" s="21"/>
       <c r="S16" s="21"/>
       <c r="T16" s="21"/>
-      <c r="U16" s="19"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U16" s="21"/>
+      <c r="V16" s="19"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
       <c r="B17" s="18"/>
       <c r="C17" s="22"/>
@@ -1191,15 +1234,16 @@
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="22"/>
       <c r="Q17" s="21"/>
       <c r="R17" s="21"/>
       <c r="S17" s="21"/>
       <c r="T17" s="21"/>
-      <c r="U17" s="19"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U17" s="21"/>
+      <c r="V17" s="19"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
       <c r="B18" s="18"/>
       <c r="C18" s="22"/>
@@ -1214,15 +1258,16 @@
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="22"/>
       <c r="Q18" s="21"/>
       <c r="R18" s="21"/>
       <c r="S18" s="21"/>
       <c r="T18" s="21"/>
-      <c r="U18" s="19"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U18" s="21"/>
+      <c r="V18" s="19"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
       <c r="B19" s="18"/>
       <c r="C19" s="22"/>
@@ -1237,15 +1282,16 @@
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="22"/>
       <c r="Q19" s="21"/>
       <c r="R19" s="21"/>
       <c r="S19" s="21"/>
       <c r="T19" s="21"/>
-      <c r="U19" s="19"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U19" s="21"/>
+      <c r="V19" s="19"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="18"/>
       <c r="C20" s="22"/>
@@ -1260,15 +1306,16 @@
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="22"/>
       <c r="Q20" s="21"/>
       <c r="R20" s="21"/>
       <c r="S20" s="21"/>
       <c r="T20" s="21"/>
-      <c r="U20" s="19"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U20" s="21"/>
+      <c r="V20" s="19"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="23"/>
       <c r="B21" s="18"/>
       <c r="C21" s="22"/>
@@ -1283,15 +1330,16 @@
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="22"/>
       <c r="Q21" s="21"/>
       <c r="R21" s="21"/>
       <c r="S21" s="21"/>
       <c r="T21" s="21"/>
-      <c r="U21" s="19"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U21" s="21"/>
+      <c r="V21" s="19"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="18"/>
       <c r="C22" s="22"/>
@@ -1306,15 +1354,16 @@
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="22"/>
       <c r="Q22" s="21"/>
       <c r="R22" s="21"/>
       <c r="S22" s="21"/>
       <c r="T22" s="21"/>
-      <c r="U22" s="19"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U22" s="21"/>
+      <c r="V22" s="19"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="23"/>
       <c r="B23" s="18"/>
       <c r="C23" s="22"/>
@@ -1329,15 +1378,16 @@
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="22"/>
       <c r="Q23" s="21"/>
       <c r="R23" s="21"/>
       <c r="S23" s="21"/>
       <c r="T23" s="21"/>
-      <c r="U23" s="19"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U23" s="21"/>
+      <c r="V23" s="19"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="18"/>
       <c r="C24" s="22"/>
@@ -1352,15 +1402,16 @@
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="22"/>
       <c r="Q24" s="21"/>
       <c r="R24" s="21"/>
       <c r="S24" s="21"/>
       <c r="T24" s="21"/>
-      <c r="U24" s="19"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U24" s="21"/>
+      <c r="V24" s="19"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="18"/>
       <c r="C25" s="22"/>
@@ -1375,15 +1426,16 @@
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="22"/>
       <c r="Q25" s="21"/>
       <c r="R25" s="21"/>
       <c r="S25" s="21"/>
       <c r="T25" s="21"/>
-      <c r="U25" s="19"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U25" s="21"/>
+      <c r="V25" s="19"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="18"/>
       <c r="C26" s="22"/>
@@ -1398,15 +1450,16 @@
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
       <c r="N26" s="21"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="22"/>
       <c r="Q26" s="21"/>
       <c r="R26" s="21"/>
       <c r="S26" s="21"/>
       <c r="T26" s="21"/>
-      <c r="U26" s="19"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U26" s="21"/>
+      <c r="V26" s="19"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="18"/>
       <c r="C27" s="22"/>
@@ -1421,15 +1474,16 @@
       <c r="L27" s="21"/>
       <c r="M27" s="21"/>
       <c r="N27" s="21"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="22"/>
       <c r="Q27" s="21"/>
       <c r="R27" s="21"/>
       <c r="S27" s="21"/>
       <c r="T27" s="21"/>
-      <c r="U27" s="19"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U27" s="21"/>
+      <c r="V27" s="19"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="18"/>
       <c r="C28" s="22"/>
@@ -1444,15 +1498,16 @@
       <c r="L28" s="21"/>
       <c r="M28" s="21"/>
       <c r="N28" s="21"/>
-      <c r="O28" s="22"/>
-      <c r="P28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="22"/>
       <c r="Q28" s="21"/>
       <c r="R28" s="21"/>
       <c r="S28" s="21"/>
       <c r="T28" s="21"/>
-      <c r="U28" s="19"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U28" s="21"/>
+      <c r="V28" s="19"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="23"/>
       <c r="B29" s="18"/>
       <c r="C29" s="22"/>
@@ -1467,15 +1522,16 @@
       <c r="L29" s="21"/>
       <c r="M29" s="21"/>
       <c r="N29" s="21"/>
-      <c r="O29" s="22"/>
-      <c r="P29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="22"/>
       <c r="Q29" s="21"/>
       <c r="R29" s="21"/>
       <c r="S29" s="21"/>
       <c r="T29" s="21"/>
-      <c r="U29" s="19"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U29" s="21"/>
+      <c r="V29" s="19"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="23"/>
       <c r="B30" s="18"/>
       <c r="C30" s="22"/>
@@ -1490,15 +1546,16 @@
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
       <c r="N30" s="21"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="22"/>
       <c r="Q30" s="21"/>
       <c r="R30" s="21"/>
       <c r="S30" s="21"/>
       <c r="T30" s="21"/>
-      <c r="U30" s="19"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U30" s="21"/>
+      <c r="V30" s="19"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="23"/>
       <c r="B31" s="18"/>
       <c r="C31" s="22"/>
@@ -1513,15 +1570,16 @@
       <c r="L31" s="21"/>
       <c r="M31" s="21"/>
       <c r="N31" s="21"/>
-      <c r="O31" s="22"/>
-      <c r="P31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="22"/>
       <c r="Q31" s="21"/>
       <c r="R31" s="21"/>
       <c r="S31" s="21"/>
       <c r="T31" s="21"/>
-      <c r="U31" s="19"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U31" s="21"/>
+      <c r="V31" s="19"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="23"/>
       <c r="B32" s="18"/>
       <c r="C32" s="22"/>
@@ -1536,15 +1594,16 @@
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
       <c r="N32" s="21"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="22"/>
       <c r="Q32" s="21"/>
       <c r="R32" s="21"/>
       <c r="S32" s="21"/>
       <c r="T32" s="21"/>
-      <c r="U32" s="19"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U32" s="21"/>
+      <c r="V32" s="19"/>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="18"/>
       <c r="C33" s="22"/>
@@ -1559,15 +1618,16 @@
       <c r="L33" s="21"/>
       <c r="M33" s="21"/>
       <c r="N33" s="21"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="22"/>
       <c r="Q33" s="21"/>
       <c r="R33" s="21"/>
       <c r="S33" s="21"/>
       <c r="T33" s="21"/>
-      <c r="U33" s="19"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U33" s="21"/>
+      <c r="V33" s="19"/>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="18"/>
       <c r="C34" s="22"/>
@@ -1582,15 +1642,16 @@
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
       <c r="N34" s="21"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="22"/>
       <c r="Q34" s="21"/>
       <c r="R34" s="21"/>
       <c r="S34" s="21"/>
       <c r="T34" s="21"/>
-      <c r="U34" s="19"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U34" s="21"/>
+      <c r="V34" s="19"/>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="18"/>
       <c r="C35" s="22"/>
@@ -1605,15 +1666,16 @@
       <c r="L35" s="21"/>
       <c r="M35" s="21"/>
       <c r="N35" s="21"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="22"/>
       <c r="Q35" s="21"/>
       <c r="R35" s="21"/>
       <c r="S35" s="21"/>
       <c r="T35" s="21"/>
-      <c r="U35" s="19"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U35" s="21"/>
+      <c r="V35" s="19"/>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
       <c r="B36" s="18"/>
       <c r="C36" s="22"/>
@@ -1628,15 +1690,16 @@
       <c r="L36" s="21"/>
       <c r="M36" s="21"/>
       <c r="N36" s="21"/>
-      <c r="O36" s="22"/>
-      <c r="P36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="22"/>
       <c r="Q36" s="21"/>
       <c r="R36" s="21"/>
       <c r="S36" s="21"/>
       <c r="T36" s="21"/>
-      <c r="U36" s="19"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U36" s="21"/>
+      <c r="V36" s="19"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
       <c r="B37" s="18"/>
       <c r="C37" s="22"/>
@@ -1651,15 +1714,16 @@
       <c r="L37" s="21"/>
       <c r="M37" s="21"/>
       <c r="N37" s="21"/>
-      <c r="O37" s="22"/>
-      <c r="P37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="22"/>
       <c r="Q37" s="21"/>
       <c r="R37" s="21"/>
       <c r="S37" s="21"/>
       <c r="T37" s="21"/>
-      <c r="U37" s="19"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U37" s="21"/>
+      <c r="V37" s="19"/>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
       <c r="B38" s="18"/>
       <c r="C38" s="22"/>
@@ -1674,15 +1738,16 @@
       <c r="L38" s="21"/>
       <c r="M38" s="21"/>
       <c r="N38" s="21"/>
-      <c r="O38" s="22"/>
-      <c r="P38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="22"/>
       <c r="Q38" s="21"/>
       <c r="R38" s="21"/>
       <c r="S38" s="21"/>
       <c r="T38" s="21"/>
-      <c r="U38" s="19"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U38" s="21"/>
+      <c r="V38" s="19"/>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="23"/>
       <c r="B39" s="18"/>
       <c r="C39" s="22"/>
@@ -1697,15 +1762,16 @@
       <c r="L39" s="21"/>
       <c r="M39" s="21"/>
       <c r="N39" s="21"/>
-      <c r="O39" s="22"/>
-      <c r="P39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="22"/>
       <c r="Q39" s="21"/>
       <c r="R39" s="21"/>
       <c r="S39" s="21"/>
       <c r="T39" s="21"/>
-      <c r="U39" s="19"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U39" s="21"/>
+      <c r="V39" s="19"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="18"/>
       <c r="C40" s="22"/>
@@ -1720,15 +1786,16 @@
       <c r="L40" s="21"/>
       <c r="M40" s="21"/>
       <c r="N40" s="21"/>
-      <c r="O40" s="22"/>
-      <c r="P40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="22"/>
       <c r="Q40" s="21"/>
       <c r="R40" s="21"/>
       <c r="S40" s="21"/>
       <c r="T40" s="21"/>
-      <c r="U40" s="19"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U40" s="21"/>
+      <c r="V40" s="19"/>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="23"/>
       <c r="B41" s="18"/>
       <c r="C41" s="22"/>
@@ -1743,15 +1810,16 @@
       <c r="L41" s="21"/>
       <c r="M41" s="21"/>
       <c r="N41" s="21"/>
-      <c r="O41" s="22"/>
-      <c r="P41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="22"/>
       <c r="Q41" s="21"/>
       <c r="R41" s="21"/>
       <c r="S41" s="21"/>
       <c r="T41" s="21"/>
-      <c r="U41" s="19"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U41" s="21"/>
+      <c r="V41" s="19"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="23"/>
       <c r="B42" s="18"/>
       <c r="C42" s="22"/>
@@ -1766,15 +1834,16 @@
       <c r="L42" s="21"/>
       <c r="M42" s="21"/>
       <c r="N42" s="21"/>
-      <c r="O42" s="22"/>
-      <c r="P42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="22"/>
       <c r="Q42" s="21"/>
       <c r="R42" s="21"/>
       <c r="S42" s="21"/>
       <c r="T42" s="21"/>
-      <c r="U42" s="19"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U42" s="21"/>
+      <c r="V42" s="19"/>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="23"/>
       <c r="B43" s="18"/>
       <c r="C43" s="22"/>
@@ -1789,15 +1858,16 @@
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
-      <c r="O43" s="22"/>
-      <c r="P43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="22"/>
       <c r="Q43" s="21"/>
       <c r="R43" s="21"/>
       <c r="S43" s="21"/>
       <c r="T43" s="21"/>
-      <c r="U43" s="19"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U43" s="21"/>
+      <c r="V43" s="19"/>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="23"/>
       <c r="B44" s="18"/>
       <c r="C44" s="22"/>
@@ -1812,15 +1882,16 @@
       <c r="L44" s="21"/>
       <c r="M44" s="21"/>
       <c r="N44" s="21"/>
-      <c r="O44" s="22"/>
-      <c r="P44" s="21"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="22"/>
       <c r="Q44" s="21"/>
       <c r="R44" s="21"/>
       <c r="S44" s="21"/>
       <c r="T44" s="21"/>
-      <c r="U44" s="19"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U44" s="21"/>
+      <c r="V44" s="19"/>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="23"/>
       <c r="B45" s="18"/>
       <c r="C45" s="22"/>
@@ -1835,15 +1906,16 @@
       <c r="L45" s="21"/>
       <c r="M45" s="21"/>
       <c r="N45" s="21"/>
-      <c r="O45" s="22"/>
-      <c r="P45" s="21"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="22"/>
       <c r="Q45" s="21"/>
       <c r="R45" s="21"/>
       <c r="S45" s="21"/>
       <c r="T45" s="21"/>
-      <c r="U45" s="19"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U45" s="21"/>
+      <c r="V45" s="19"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="23"/>
       <c r="B46" s="18"/>
       <c r="C46" s="22"/>
@@ -1858,15 +1930,16 @@
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
-      <c r="O46" s="22"/>
-      <c r="P46" s="21"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="22"/>
       <c r="Q46" s="21"/>
       <c r="R46" s="21"/>
       <c r="S46" s="21"/>
       <c r="T46" s="21"/>
-      <c r="U46" s="19"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U46" s="21"/>
+      <c r="V46" s="19"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
       <c r="B47" s="18"/>
       <c r="C47" s="22"/>
@@ -1881,15 +1954,16 @@
       <c r="L47" s="21"/>
       <c r="M47" s="21"/>
       <c r="N47" s="21"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="21"/>
+      <c r="O47" s="21"/>
+      <c r="P47" s="22"/>
       <c r="Q47" s="21"/>
       <c r="R47" s="21"/>
       <c r="S47" s="21"/>
       <c r="T47" s="21"/>
-      <c r="U47" s="19"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U47" s="21"/>
+      <c r="V47" s="19"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="23"/>
       <c r="B48" s="18"/>
       <c r="C48" s="22"/>
@@ -1904,15 +1978,16 @@
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
-      <c r="O48" s="22"/>
-      <c r="P48" s="21"/>
+      <c r="O48" s="21"/>
+      <c r="P48" s="22"/>
       <c r="Q48" s="21"/>
       <c r="R48" s="21"/>
       <c r="S48" s="21"/>
       <c r="T48" s="21"/>
-      <c r="U48" s="19"/>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U48" s="21"/>
+      <c r="V48" s="19"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="18"/>
       <c r="C49" s="22"/>
@@ -1927,15 +2002,16 @@
       <c r="L49" s="21"/>
       <c r="M49" s="21"/>
       <c r="N49" s="21"/>
-      <c r="O49" s="22"/>
-      <c r="P49" s="21"/>
+      <c r="O49" s="21"/>
+      <c r="P49" s="22"/>
       <c r="Q49" s="21"/>
       <c r="R49" s="21"/>
       <c r="S49" s="21"/>
       <c r="T49" s="21"/>
-      <c r="U49" s="19"/>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U49" s="21"/>
+      <c r="V49" s="19"/>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
       <c r="B50" s="18"/>
       <c r="C50" s="22"/>
@@ -1950,15 +2026,16 @@
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
-      <c r="O50" s="22"/>
-      <c r="P50" s="21"/>
+      <c r="O50" s="21"/>
+      <c r="P50" s="22"/>
       <c r="Q50" s="21"/>
       <c r="R50" s="21"/>
       <c r="S50" s="21"/>
       <c r="T50" s="21"/>
-      <c r="U50" s="19"/>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U50" s="21"/>
+      <c r="V50" s="19"/>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>
       <c r="B51" s="18"/>
       <c r="C51" s="22"/>
@@ -1973,15 +2050,16 @@
       <c r="L51" s="21"/>
       <c r="M51" s="21"/>
       <c r="N51" s="21"/>
-      <c r="O51" s="22"/>
-      <c r="P51" s="21"/>
+      <c r="O51" s="21"/>
+      <c r="P51" s="22"/>
       <c r="Q51" s="21"/>
       <c r="R51" s="21"/>
       <c r="S51" s="21"/>
       <c r="T51" s="21"/>
-      <c r="U51" s="19"/>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U51" s="21"/>
+      <c r="V51" s="19"/>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="18"/>
       <c r="C52" s="22"/>
@@ -1996,15 +2074,16 @@
       <c r="L52" s="21"/>
       <c r="M52" s="21"/>
       <c r="N52" s="21"/>
-      <c r="O52" s="22"/>
-      <c r="P52" s="21"/>
+      <c r="O52" s="21"/>
+      <c r="P52" s="22"/>
       <c r="Q52" s="21"/>
       <c r="R52" s="21"/>
       <c r="S52" s="21"/>
       <c r="T52" s="21"/>
-      <c r="U52" s="19"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U52" s="21"/>
+      <c r="V52" s="19"/>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
       <c r="B53" s="18"/>
       <c r="C53" s="22"/>
@@ -2019,15 +2098,16 @@
       <c r="L53" s="21"/>
       <c r="M53" s="21"/>
       <c r="N53" s="21"/>
-      <c r="O53" s="22"/>
-      <c r="P53" s="21"/>
+      <c r="O53" s="21"/>
+      <c r="P53" s="22"/>
       <c r="Q53" s="21"/>
       <c r="R53" s="21"/>
       <c r="S53" s="21"/>
       <c r="T53" s="21"/>
-      <c r="U53" s="19"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U53" s="21"/>
+      <c r="V53" s="19"/>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="18"/>
       <c r="C54" s="22"/>
@@ -2042,15 +2122,16 @@
       <c r="L54" s="21"/>
       <c r="M54" s="21"/>
       <c r="N54" s="21"/>
-      <c r="O54" s="22"/>
-      <c r="P54" s="21"/>
+      <c r="O54" s="21"/>
+      <c r="P54" s="22"/>
       <c r="Q54" s="21"/>
       <c r="R54" s="21"/>
       <c r="S54" s="21"/>
       <c r="T54" s="21"/>
-      <c r="U54" s="19"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U54" s="21"/>
+      <c r="V54" s="19"/>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
       <c r="B55" s="18"/>
       <c r="C55" s="22"/>
@@ -2065,15 +2146,16 @@
       <c r="L55" s="21"/>
       <c r="M55" s="21"/>
       <c r="N55" s="21"/>
-      <c r="O55" s="22"/>
-      <c r="P55" s="21"/>
+      <c r="O55" s="21"/>
+      <c r="P55" s="22"/>
       <c r="Q55" s="21"/>
       <c r="R55" s="21"/>
       <c r="S55" s="21"/>
       <c r="T55" s="21"/>
-      <c r="U55" s="19"/>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U55" s="21"/>
+      <c r="V55" s="19"/>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="23"/>
       <c r="B56" s="18"/>
       <c r="C56" s="22"/>
@@ -2088,15 +2170,16 @@
       <c r="L56" s="21"/>
       <c r="M56" s="21"/>
       <c r="N56" s="21"/>
-      <c r="O56" s="22"/>
-      <c r="P56" s="21"/>
+      <c r="O56" s="21"/>
+      <c r="P56" s="22"/>
       <c r="Q56" s="21"/>
       <c r="R56" s="21"/>
       <c r="S56" s="21"/>
       <c r="T56" s="21"/>
-      <c r="U56" s="19"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U56" s="21"/>
+      <c r="V56" s="19"/>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="23"/>
       <c r="B57" s="18"/>
       <c r="C57" s="22"/>
@@ -2111,15 +2194,16 @@
       <c r="L57" s="21"/>
       <c r="M57" s="21"/>
       <c r="N57" s="21"/>
-      <c r="O57" s="22"/>
-      <c r="P57" s="21"/>
+      <c r="O57" s="21"/>
+      <c r="P57" s="22"/>
       <c r="Q57" s="21"/>
       <c r="R57" s="21"/>
       <c r="S57" s="21"/>
       <c r="T57" s="21"/>
-      <c r="U57" s="19"/>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U57" s="21"/>
+      <c r="V57" s="19"/>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="23"/>
       <c r="B58" s="18"/>
       <c r="C58" s="22"/>
@@ -2134,15 +2218,16 @@
       <c r="L58" s="21"/>
       <c r="M58" s="21"/>
       <c r="N58" s="21"/>
-      <c r="O58" s="22"/>
-      <c r="P58" s="21"/>
+      <c r="O58" s="21"/>
+      <c r="P58" s="22"/>
       <c r="Q58" s="21"/>
       <c r="R58" s="21"/>
       <c r="S58" s="21"/>
       <c r="T58" s="21"/>
-      <c r="U58" s="19"/>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U58" s="21"/>
+      <c r="V58" s="19"/>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="23"/>
       <c r="B59" s="18"/>
       <c r="C59" s="22"/>
@@ -2157,15 +2242,16 @@
       <c r="L59" s="21"/>
       <c r="M59" s="21"/>
       <c r="N59" s="21"/>
-      <c r="O59" s="22"/>
-      <c r="P59" s="21"/>
+      <c r="O59" s="21"/>
+      <c r="P59" s="22"/>
       <c r="Q59" s="21"/>
       <c r="R59" s="21"/>
       <c r="S59" s="21"/>
       <c r="T59" s="21"/>
-      <c r="U59" s="19"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U59" s="21"/>
+      <c r="V59" s="19"/>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
       <c r="B60" s="18"/>
       <c r="C60" s="22"/>
@@ -2180,15 +2266,16 @@
       <c r="L60" s="21"/>
       <c r="M60" s="21"/>
       <c r="N60" s="21"/>
-      <c r="O60" s="22"/>
-      <c r="P60" s="21"/>
+      <c r="O60" s="21"/>
+      <c r="P60" s="22"/>
       <c r="Q60" s="21"/>
       <c r="R60" s="21"/>
       <c r="S60" s="21"/>
       <c r="T60" s="21"/>
-      <c r="U60" s="19"/>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U60" s="21"/>
+      <c r="V60" s="19"/>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="23"/>
       <c r="B61" s="18"/>
       <c r="C61" s="22"/>
@@ -2203,15 +2290,16 @@
       <c r="L61" s="21"/>
       <c r="M61" s="21"/>
       <c r="N61" s="21"/>
-      <c r="O61" s="22"/>
-      <c r="P61" s="21"/>
+      <c r="O61" s="21"/>
+      <c r="P61" s="22"/>
       <c r="Q61" s="21"/>
       <c r="R61" s="21"/>
       <c r="S61" s="21"/>
       <c r="T61" s="21"/>
-      <c r="U61" s="19"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U61" s="21"/>
+      <c r="V61" s="19"/>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="23"/>
       <c r="B62" s="18"/>
       <c r="C62" s="22"/>
@@ -2226,15 +2314,16 @@
       <c r="L62" s="21"/>
       <c r="M62" s="21"/>
       <c r="N62" s="21"/>
-      <c r="O62" s="22"/>
-      <c r="P62" s="21"/>
+      <c r="O62" s="21"/>
+      <c r="P62" s="22"/>
       <c r="Q62" s="21"/>
       <c r="R62" s="21"/>
       <c r="S62" s="21"/>
       <c r="T62" s="21"/>
-      <c r="U62" s="19"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U62" s="21"/>
+      <c r="V62" s="19"/>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="23"/>
       <c r="B63" s="18"/>
       <c r="C63" s="22"/>
@@ -2249,15 +2338,16 @@
       <c r="L63" s="21"/>
       <c r="M63" s="21"/>
       <c r="N63" s="21"/>
-      <c r="O63" s="22"/>
-      <c r="P63" s="21"/>
+      <c r="O63" s="21"/>
+      <c r="P63" s="22"/>
       <c r="Q63" s="21"/>
       <c r="R63" s="21"/>
       <c r="S63" s="21"/>
       <c r="T63" s="21"/>
-      <c r="U63" s="19"/>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U63" s="21"/>
+      <c r="V63" s="19"/>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="23"/>
       <c r="B64" s="18"/>
       <c r="C64" s="22"/>
@@ -2272,15 +2362,16 @@
       <c r="L64" s="21"/>
       <c r="M64" s="21"/>
       <c r="N64" s="21"/>
-      <c r="O64" s="22"/>
-      <c r="P64" s="21"/>
+      <c r="O64" s="21"/>
+      <c r="P64" s="22"/>
       <c r="Q64" s="21"/>
       <c r="R64" s="21"/>
       <c r="S64" s="21"/>
       <c r="T64" s="21"/>
-      <c r="U64" s="19"/>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U64" s="21"/>
+      <c r="V64" s="19"/>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="23"/>
       <c r="B65" s="18"/>
       <c r="C65" s="22"/>
@@ -2295,15 +2386,16 @@
       <c r="L65" s="21"/>
       <c r="M65" s="21"/>
       <c r="N65" s="21"/>
-      <c r="O65" s="22"/>
-      <c r="P65" s="21"/>
+      <c r="O65" s="21"/>
+      <c r="P65" s="22"/>
       <c r="Q65" s="21"/>
       <c r="R65" s="21"/>
       <c r="S65" s="21"/>
       <c r="T65" s="21"/>
-      <c r="U65" s="19"/>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U65" s="21"/>
+      <c r="V65" s="19"/>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="23"/>
       <c r="B66" s="18"/>
       <c r="C66" s="22"/>
@@ -2318,15 +2410,16 @@
       <c r="L66" s="21"/>
       <c r="M66" s="21"/>
       <c r="N66" s="21"/>
-      <c r="O66" s="22"/>
-      <c r="P66" s="21"/>
+      <c r="O66" s="21"/>
+      <c r="P66" s="22"/>
       <c r="Q66" s="21"/>
       <c r="R66" s="21"/>
       <c r="S66" s="21"/>
       <c r="T66" s="21"/>
-      <c r="U66" s="19"/>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U66" s="21"/>
+      <c r="V66" s="19"/>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="23"/>
       <c r="B67" s="18"/>
       <c r="C67" s="22"/>
@@ -2341,15 +2434,16 @@
       <c r="L67" s="21"/>
       <c r="M67" s="21"/>
       <c r="N67" s="21"/>
-      <c r="O67" s="22"/>
-      <c r="P67" s="21"/>
+      <c r="O67" s="21"/>
+      <c r="P67" s="22"/>
       <c r="Q67" s="21"/>
       <c r="R67" s="21"/>
       <c r="S67" s="21"/>
       <c r="T67" s="21"/>
-      <c r="U67" s="19"/>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U67" s="21"/>
+      <c r="V67" s="19"/>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="23"/>
       <c r="B68" s="18"/>
       <c r="C68" s="22"/>
@@ -2364,15 +2458,16 @@
       <c r="L68" s="21"/>
       <c r="M68" s="21"/>
       <c r="N68" s="21"/>
-      <c r="O68" s="22"/>
-      <c r="P68" s="21"/>
+      <c r="O68" s="21"/>
+      <c r="P68" s="22"/>
       <c r="Q68" s="21"/>
       <c r="R68" s="21"/>
       <c r="S68" s="21"/>
       <c r="T68" s="21"/>
-      <c r="U68" s="19"/>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U68" s="21"/>
+      <c r="V68" s="19"/>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="23"/>
       <c r="B69" s="18"/>
       <c r="C69" s="22"/>
@@ -2387,15 +2482,16 @@
       <c r="L69" s="21"/>
       <c r="M69" s="21"/>
       <c r="N69" s="21"/>
-      <c r="O69" s="22"/>
-      <c r="P69" s="21"/>
+      <c r="O69" s="21"/>
+      <c r="P69" s="22"/>
       <c r="Q69" s="21"/>
       <c r="R69" s="21"/>
       <c r="S69" s="21"/>
       <c r="T69" s="21"/>
-      <c r="U69" s="19"/>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U69" s="21"/>
+      <c r="V69" s="19"/>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="23"/>
       <c r="B70" s="18"/>
       <c r="C70" s="22"/>
@@ -2410,15 +2506,16 @@
       <c r="L70" s="21"/>
       <c r="M70" s="21"/>
       <c r="N70" s="21"/>
-      <c r="O70" s="22"/>
-      <c r="P70" s="21"/>
+      <c r="O70" s="21"/>
+      <c r="P70" s="22"/>
       <c r="Q70" s="21"/>
       <c r="R70" s="21"/>
       <c r="S70" s="21"/>
       <c r="T70" s="21"/>
-      <c r="U70" s="19"/>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U70" s="21"/>
+      <c r="V70" s="19"/>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="23"/>
       <c r="B71" s="18"/>
       <c r="C71" s="22"/>
@@ -2433,15 +2530,16 @@
       <c r="L71" s="21"/>
       <c r="M71" s="21"/>
       <c r="N71" s="21"/>
-      <c r="O71" s="22"/>
-      <c r="P71" s="21"/>
+      <c r="O71" s="21"/>
+      <c r="P71" s="22"/>
       <c r="Q71" s="21"/>
       <c r="R71" s="21"/>
       <c r="S71" s="21"/>
       <c r="T71" s="21"/>
-      <c r="U71" s="19"/>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U71" s="21"/>
+      <c r="V71" s="19"/>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="23"/>
       <c r="B72" s="18"/>
       <c r="C72" s="22"/>
@@ -2456,15 +2554,16 @@
       <c r="L72" s="21"/>
       <c r="M72" s="21"/>
       <c r="N72" s="21"/>
-      <c r="O72" s="22"/>
-      <c r="P72" s="21"/>
+      <c r="O72" s="21"/>
+      <c r="P72" s="22"/>
       <c r="Q72" s="21"/>
       <c r="R72" s="21"/>
       <c r="S72" s="21"/>
       <c r="T72" s="21"/>
-      <c r="U72" s="19"/>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U72" s="21"/>
+      <c r="V72" s="19"/>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="23"/>
       <c r="B73" s="18"/>
       <c r="C73" s="22"/>
@@ -2479,15 +2578,16 @@
       <c r="L73" s="21"/>
       <c r="M73" s="21"/>
       <c r="N73" s="21"/>
-      <c r="O73" s="22"/>
-      <c r="P73" s="21"/>
+      <c r="O73" s="21"/>
+      <c r="P73" s="22"/>
       <c r="Q73" s="21"/>
       <c r="R73" s="21"/>
       <c r="S73" s="21"/>
       <c r="T73" s="21"/>
-      <c r="U73" s="19"/>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U73" s="21"/>
+      <c r="V73" s="19"/>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="23"/>
       <c r="B74" s="18"/>
       <c r="C74" s="22"/>
@@ -2502,15 +2602,16 @@
       <c r="L74" s="21"/>
       <c r="M74" s="21"/>
       <c r="N74" s="21"/>
-      <c r="O74" s="22"/>
-      <c r="P74" s="21"/>
+      <c r="O74" s="21"/>
+      <c r="P74" s="22"/>
       <c r="Q74" s="21"/>
       <c r="R74" s="21"/>
       <c r="S74" s="21"/>
       <c r="T74" s="21"/>
-      <c r="U74" s="19"/>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U74" s="21"/>
+      <c r="V74" s="19"/>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="23"/>
       <c r="B75" s="18"/>
       <c r="C75" s="22"/>
@@ -2525,15 +2626,16 @@
       <c r="L75" s="21"/>
       <c r="M75" s="21"/>
       <c r="N75" s="21"/>
-      <c r="O75" s="22"/>
-      <c r="P75" s="21"/>
+      <c r="O75" s="21"/>
+      <c r="P75" s="22"/>
       <c r="Q75" s="21"/>
       <c r="R75" s="21"/>
       <c r="S75" s="21"/>
       <c r="T75" s="21"/>
-      <c r="U75" s="19"/>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U75" s="21"/>
+      <c r="V75" s="19"/>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="23"/>
       <c r="B76" s="18"/>
       <c r="C76" s="22"/>
@@ -2548,15 +2650,16 @@
       <c r="L76" s="21"/>
       <c r="M76" s="21"/>
       <c r="N76" s="21"/>
-      <c r="O76" s="22"/>
-      <c r="P76" s="21"/>
+      <c r="O76" s="21"/>
+      <c r="P76" s="22"/>
       <c r="Q76" s="21"/>
       <c r="R76" s="21"/>
       <c r="S76" s="21"/>
       <c r="T76" s="21"/>
-      <c r="U76" s="19"/>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U76" s="21"/>
+      <c r="V76" s="19"/>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="23"/>
       <c r="B77" s="18"/>
       <c r="C77" s="22"/>
@@ -2571,15 +2674,16 @@
       <c r="L77" s="21"/>
       <c r="M77" s="21"/>
       <c r="N77" s="21"/>
-      <c r="O77" s="22"/>
-      <c r="P77" s="21"/>
+      <c r="O77" s="21"/>
+      <c r="P77" s="22"/>
       <c r="Q77" s="21"/>
       <c r="R77" s="21"/>
       <c r="S77" s="21"/>
       <c r="T77" s="21"/>
-      <c r="U77" s="19"/>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U77" s="21"/>
+      <c r="V77" s="19"/>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" s="23"/>
       <c r="B78" s="18"/>
       <c r="C78" s="22"/>
@@ -2594,15 +2698,16 @@
       <c r="L78" s="21"/>
       <c r="M78" s="21"/>
       <c r="N78" s="21"/>
-      <c r="O78" s="22"/>
-      <c r="P78" s="21"/>
+      <c r="O78" s="21"/>
+      <c r="P78" s="22"/>
       <c r="Q78" s="21"/>
       <c r="R78" s="21"/>
       <c r="S78" s="21"/>
       <c r="T78" s="21"/>
-      <c r="U78" s="19"/>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U78" s="21"/>
+      <c r="V78" s="19"/>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" s="23"/>
       <c r="B79" s="18"/>
       <c r="C79" s="22"/>
@@ -2617,15 +2722,16 @@
       <c r="L79" s="21"/>
       <c r="M79" s="21"/>
       <c r="N79" s="21"/>
-      <c r="O79" s="22"/>
-      <c r="P79" s="21"/>
+      <c r="O79" s="21"/>
+      <c r="P79" s="22"/>
       <c r="Q79" s="21"/>
       <c r="R79" s="21"/>
       <c r="S79" s="21"/>
       <c r="T79" s="21"/>
-      <c r="U79" s="19"/>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U79" s="21"/>
+      <c r="V79" s="19"/>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="23"/>
       <c r="B80" s="18"/>
       <c r="C80" s="22"/>
@@ -2640,15 +2746,16 @@
       <c r="L80" s="21"/>
       <c r="M80" s="21"/>
       <c r="N80" s="21"/>
-      <c r="O80" s="22"/>
-      <c r="P80" s="21"/>
+      <c r="O80" s="21"/>
+      <c r="P80" s="22"/>
       <c r="Q80" s="21"/>
       <c r="R80" s="21"/>
       <c r="S80" s="21"/>
       <c r="T80" s="21"/>
-      <c r="U80" s="19"/>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U80" s="21"/>
+      <c r="V80" s="19"/>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" s="23"/>
       <c r="B81" s="18"/>
       <c r="C81" s="22"/>
@@ -2663,15 +2770,16 @@
       <c r="L81" s="21"/>
       <c r="M81" s="21"/>
       <c r="N81" s="21"/>
-      <c r="O81" s="22"/>
-      <c r="P81" s="21"/>
+      <c r="O81" s="21"/>
+      <c r="P81" s="22"/>
       <c r="Q81" s="21"/>
       <c r="R81" s="21"/>
       <c r="S81" s="21"/>
       <c r="T81" s="21"/>
-      <c r="U81" s="19"/>
-    </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U81" s="21"/>
+      <c r="V81" s="19"/>
+    </row>
+    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A82" s="23"/>
       <c r="B82" s="18"/>
       <c r="C82" s="22"/>
@@ -2686,15 +2794,16 @@
       <c r="L82" s="21"/>
       <c r="M82" s="21"/>
       <c r="N82" s="21"/>
-      <c r="O82" s="22"/>
-      <c r="P82" s="21"/>
+      <c r="O82" s="21"/>
+      <c r="P82" s="22"/>
       <c r="Q82" s="21"/>
       <c r="R82" s="21"/>
       <c r="S82" s="21"/>
       <c r="T82" s="21"/>
-      <c r="U82" s="19"/>
-    </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U82" s="21"/>
+      <c r="V82" s="19"/>
+    </row>
+    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A83" s="23"/>
       <c r="B83" s="18"/>
       <c r="C83" s="22"/>
@@ -2709,15 +2818,16 @@
       <c r="L83" s="21"/>
       <c r="M83" s="21"/>
       <c r="N83" s="21"/>
-      <c r="O83" s="22"/>
-      <c r="P83" s="21"/>
+      <c r="O83" s="21"/>
+      <c r="P83" s="22"/>
       <c r="Q83" s="21"/>
       <c r="R83" s="21"/>
       <c r="S83" s="21"/>
       <c r="T83" s="21"/>
-      <c r="U83" s="19"/>
-    </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U83" s="21"/>
+      <c r="V83" s="19"/>
+    </row>
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A84" s="23"/>
       <c r="B84" s="18"/>
       <c r="C84" s="22"/>
@@ -2732,15 +2842,16 @@
       <c r="L84" s="21"/>
       <c r="M84" s="21"/>
       <c r="N84" s="21"/>
-      <c r="O84" s="22"/>
-      <c r="P84" s="21"/>
+      <c r="O84" s="21"/>
+      <c r="P84" s="22"/>
       <c r="Q84" s="21"/>
       <c r="R84" s="21"/>
       <c r="S84" s="21"/>
       <c r="T84" s="21"/>
-      <c r="U84" s="19"/>
-    </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U84" s="21"/>
+      <c r="V84" s="19"/>
+    </row>
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A85" s="23"/>
       <c r="B85" s="18"/>
       <c r="C85" s="22"/>
@@ -2755,15 +2866,16 @@
       <c r="L85" s="21"/>
       <c r="M85" s="21"/>
       <c r="N85" s="21"/>
-      <c r="O85" s="22"/>
-      <c r="P85" s="21"/>
+      <c r="O85" s="21"/>
+      <c r="P85" s="22"/>
       <c r="Q85" s="21"/>
       <c r="R85" s="21"/>
       <c r="S85" s="21"/>
       <c r="T85" s="21"/>
-      <c r="U85" s="19"/>
-    </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U85" s="21"/>
+      <c r="V85" s="19"/>
+    </row>
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A86" s="23"/>
       <c r="B86" s="18"/>
       <c r="C86" s="22"/>
@@ -2778,15 +2890,16 @@
       <c r="L86" s="21"/>
       <c r="M86" s="21"/>
       <c r="N86" s="21"/>
-      <c r="O86" s="22"/>
-      <c r="P86" s="21"/>
+      <c r="O86" s="21"/>
+      <c r="P86" s="22"/>
       <c r="Q86" s="21"/>
       <c r="R86" s="21"/>
       <c r="S86" s="21"/>
       <c r="T86" s="21"/>
-      <c r="U86" s="19"/>
-    </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U86" s="21"/>
+      <c r="V86" s="19"/>
+    </row>
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A87" s="23"/>
       <c r="B87" s="18"/>
       <c r="C87" s="22"/>
@@ -2801,15 +2914,16 @@
       <c r="L87" s="21"/>
       <c r="M87" s="21"/>
       <c r="N87" s="21"/>
-      <c r="O87" s="22"/>
-      <c r="P87" s="21"/>
+      <c r="O87" s="21"/>
+      <c r="P87" s="22"/>
       <c r="Q87" s="21"/>
       <c r="R87" s="21"/>
       <c r="S87" s="21"/>
       <c r="T87" s="21"/>
-      <c r="U87" s="19"/>
-    </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U87" s="21"/>
+      <c r="V87" s="19"/>
+    </row>
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A88" s="23"/>
       <c r="B88" s="18"/>
       <c r="C88" s="22"/>
@@ -2824,15 +2938,16 @@
       <c r="L88" s="21"/>
       <c r="M88" s="21"/>
       <c r="N88" s="21"/>
-      <c r="O88" s="22"/>
-      <c r="P88" s="21"/>
+      <c r="O88" s="21"/>
+      <c r="P88" s="22"/>
       <c r="Q88" s="21"/>
       <c r="R88" s="21"/>
       <c r="S88" s="21"/>
       <c r="T88" s="21"/>
-      <c r="U88" s="19"/>
-    </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U88" s="21"/>
+      <c r="V88" s="19"/>
+    </row>
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A89" s="23"/>
       <c r="B89" s="18"/>
       <c r="C89" s="22"/>
@@ -2847,15 +2962,16 @@
       <c r="L89" s="21"/>
       <c r="M89" s="21"/>
       <c r="N89" s="21"/>
-      <c r="O89" s="22"/>
-      <c r="P89" s="21"/>
+      <c r="O89" s="21"/>
+      <c r="P89" s="22"/>
       <c r="Q89" s="21"/>
       <c r="R89" s="21"/>
       <c r="S89" s="21"/>
       <c r="T89" s="21"/>
-      <c r="U89" s="19"/>
-    </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U89" s="21"/>
+      <c r="V89" s="19"/>
+    </row>
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A90" s="23"/>
       <c r="B90" s="18"/>
       <c r="C90" s="22"/>
@@ -2870,15 +2986,16 @@
       <c r="L90" s="21"/>
       <c r="M90" s="21"/>
       <c r="N90" s="21"/>
-      <c r="O90" s="22"/>
-      <c r="P90" s="21"/>
+      <c r="O90" s="21"/>
+      <c r="P90" s="22"/>
       <c r="Q90" s="21"/>
       <c r="R90" s="21"/>
       <c r="S90" s="21"/>
       <c r="T90" s="21"/>
-      <c r="U90" s="19"/>
-    </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U90" s="21"/>
+      <c r="V90" s="19"/>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A91" s="23"/>
       <c r="B91" s="18"/>
       <c r="C91" s="22"/>
@@ -2893,15 +3010,16 @@
       <c r="L91" s="21"/>
       <c r="M91" s="21"/>
       <c r="N91" s="21"/>
-      <c r="O91" s="22"/>
-      <c r="P91" s="21"/>
+      <c r="O91" s="21"/>
+      <c r="P91" s="22"/>
       <c r="Q91" s="21"/>
       <c r="R91" s="21"/>
       <c r="S91" s="21"/>
       <c r="T91" s="21"/>
-      <c r="U91" s="19"/>
-    </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U91" s="21"/>
+      <c r="V91" s="19"/>
+    </row>
+    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A92" s="23"/>
       <c r="B92" s="18"/>
       <c r="C92" s="22"/>
@@ -2916,15 +3034,16 @@
       <c r="L92" s="21"/>
       <c r="M92" s="21"/>
       <c r="N92" s="21"/>
-      <c r="O92" s="22"/>
-      <c r="P92" s="21"/>
+      <c r="O92" s="21"/>
+      <c r="P92" s="22"/>
       <c r="Q92" s="21"/>
       <c r="R92" s="21"/>
       <c r="S92" s="21"/>
       <c r="T92" s="21"/>
-      <c r="U92" s="19"/>
-    </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U92" s="21"/>
+      <c r="V92" s="19"/>
+    </row>
+    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A93" s="23"/>
       <c r="B93" s="18"/>
       <c r="C93" s="22"/>
@@ -2939,15 +3058,16 @@
       <c r="L93" s="21"/>
       <c r="M93" s="21"/>
       <c r="N93" s="21"/>
-      <c r="O93" s="22"/>
-      <c r="P93" s="21"/>
+      <c r="O93" s="21"/>
+      <c r="P93" s="22"/>
       <c r="Q93" s="21"/>
       <c r="R93" s="21"/>
       <c r="S93" s="21"/>
       <c r="T93" s="21"/>
-      <c r="U93" s="19"/>
-    </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U93" s="21"/>
+      <c r="V93" s="19"/>
+    </row>
+    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A94" s="23"/>
       <c r="B94" s="18"/>
       <c r="C94" s="22"/>
@@ -2962,15 +3082,16 @@
       <c r="L94" s="21"/>
       <c r="M94" s="21"/>
       <c r="N94" s="21"/>
-      <c r="O94" s="22"/>
-      <c r="P94" s="21"/>
+      <c r="O94" s="21"/>
+      <c r="P94" s="22"/>
       <c r="Q94" s="21"/>
       <c r="R94" s="21"/>
       <c r="S94" s="21"/>
       <c r="T94" s="21"/>
-      <c r="U94" s="19"/>
-    </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U94" s="21"/>
+      <c r="V94" s="19"/>
+    </row>
+    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A95" s="23"/>
       <c r="B95" s="18"/>
       <c r="C95" s="22"/>
@@ -2985,15 +3106,16 @@
       <c r="L95" s="21"/>
       <c r="M95" s="21"/>
       <c r="N95" s="21"/>
-      <c r="O95" s="22"/>
-      <c r="P95" s="21"/>
+      <c r="O95" s="21"/>
+      <c r="P95" s="22"/>
       <c r="Q95" s="21"/>
       <c r="R95" s="21"/>
       <c r="S95" s="21"/>
       <c r="T95" s="21"/>
-      <c r="U95" s="19"/>
-    </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U95" s="21"/>
+      <c r="V95" s="19"/>
+    </row>
+    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A96" s="23"/>
       <c r="B96" s="18"/>
       <c r="C96" s="22"/>
@@ -3008,15 +3130,16 @@
       <c r="L96" s="21"/>
       <c r="M96" s="21"/>
       <c r="N96" s="21"/>
-      <c r="O96" s="22"/>
-      <c r="P96" s="21"/>
+      <c r="O96" s="21"/>
+      <c r="P96" s="22"/>
       <c r="Q96" s="21"/>
       <c r="R96" s="21"/>
       <c r="S96" s="21"/>
       <c r="T96" s="21"/>
-      <c r="U96" s="19"/>
-    </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U96" s="21"/>
+      <c r="V96" s="19"/>
+    </row>
+    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A97" s="23"/>
       <c r="B97" s="18"/>
       <c r="C97" s="22"/>
@@ -3031,15 +3154,16 @@
       <c r="L97" s="21"/>
       <c r="M97" s="21"/>
       <c r="N97" s="21"/>
-      <c r="O97" s="22"/>
-      <c r="P97" s="21"/>
+      <c r="O97" s="21"/>
+      <c r="P97" s="22"/>
       <c r="Q97" s="21"/>
       <c r="R97" s="21"/>
       <c r="S97" s="21"/>
       <c r="T97" s="21"/>
-      <c r="U97" s="19"/>
-    </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U97" s="21"/>
+      <c r="V97" s="19"/>
+    </row>
+    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A98" s="23"/>
       <c r="B98" s="18"/>
       <c r="C98" s="22"/>
@@ -3054,15 +3178,16 @@
       <c r="L98" s="21"/>
       <c r="M98" s="21"/>
       <c r="N98" s="21"/>
-      <c r="O98" s="22"/>
-      <c r="P98" s="21"/>
+      <c r="O98" s="21"/>
+      <c r="P98" s="22"/>
       <c r="Q98" s="21"/>
       <c r="R98" s="21"/>
       <c r="S98" s="21"/>
       <c r="T98" s="21"/>
-      <c r="U98" s="19"/>
-    </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U98" s="21"/>
+      <c r="V98" s="19"/>
+    </row>
+    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A99" s="23"/>
       <c r="B99" s="18"/>
       <c r="C99" s="22"/>
@@ -3077,15 +3202,16 @@
       <c r="L99" s="21"/>
       <c r="M99" s="21"/>
       <c r="N99" s="21"/>
-      <c r="O99" s="22"/>
-      <c r="P99" s="21"/>
+      <c r="O99" s="21"/>
+      <c r="P99" s="22"/>
       <c r="Q99" s="21"/>
       <c r="R99" s="21"/>
       <c r="S99" s="21"/>
       <c r="T99" s="21"/>
-      <c r="U99" s="19"/>
-    </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U99" s="21"/>
+      <c r="V99" s="19"/>
+    </row>
+    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A100" s="23"/>
       <c r="B100" s="18"/>
       <c r="C100" s="22"/>
@@ -3100,15 +3226,16 @@
       <c r="L100" s="21"/>
       <c r="M100" s="21"/>
       <c r="N100" s="21"/>
-      <c r="O100" s="22"/>
-      <c r="P100" s="21"/>
+      <c r="O100" s="21"/>
+      <c r="P100" s="22"/>
       <c r="Q100" s="21"/>
       <c r="R100" s="21"/>
       <c r="S100" s="21"/>
       <c r="T100" s="21"/>
-      <c r="U100" s="19"/>
-    </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U100" s="21"/>
+      <c r="V100" s="19"/>
+    </row>
+    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A101" s="23"/>
       <c r="B101" s="18"/>
       <c r="C101" s="22"/>
@@ -3123,15 +3250,16 @@
       <c r="L101" s="21"/>
       <c r="M101" s="21"/>
       <c r="N101" s="21"/>
-      <c r="O101" s="22"/>
-      <c r="P101" s="21"/>
+      <c r="O101" s="21"/>
+      <c r="P101" s="22"/>
       <c r="Q101" s="21"/>
       <c r="R101" s="21"/>
       <c r="S101" s="21"/>
       <c r="T101" s="21"/>
-      <c r="U101" s="19"/>
-    </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U101" s="21"/>
+      <c r="V101" s="19"/>
+    </row>
+    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A102" s="23"/>
       <c r="B102" s="18"/>
       <c r="C102" s="22"/>
@@ -3146,15 +3274,16 @@
       <c r="L102" s="21"/>
       <c r="M102" s="21"/>
       <c r="N102" s="21"/>
-      <c r="O102" s="22"/>
-      <c r="P102" s="21"/>
+      <c r="O102" s="21"/>
+      <c r="P102" s="22"/>
       <c r="Q102" s="21"/>
       <c r="R102" s="21"/>
       <c r="S102" s="21"/>
       <c r="T102" s="21"/>
-      <c r="U102" s="19"/>
-    </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U102" s="21"/>
+      <c r="V102" s="19"/>
+    </row>
+    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A103" s="23"/>
       <c r="B103" s="18"/>
       <c r="C103" s="22"/>
@@ -3169,15 +3298,16 @@
       <c r="L103" s="21"/>
       <c r="M103" s="21"/>
       <c r="N103" s="21"/>
-      <c r="O103" s="22"/>
-      <c r="P103" s="21"/>
+      <c r="O103" s="21"/>
+      <c r="P103" s="22"/>
       <c r="Q103" s="21"/>
       <c r="R103" s="21"/>
       <c r="S103" s="21"/>
       <c r="T103" s="21"/>
-      <c r="U103" s="19"/>
-    </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U103" s="21"/>
+      <c r="V103" s="19"/>
+    </row>
+    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A104" s="23"/>
       <c r="B104" s="18"/>
       <c r="C104" s="22"/>
@@ -3192,15 +3322,16 @@
       <c r="L104" s="21"/>
       <c r="M104" s="21"/>
       <c r="N104" s="21"/>
-      <c r="O104" s="22"/>
-      <c r="P104" s="21"/>
+      <c r="O104" s="21"/>
+      <c r="P104" s="22"/>
       <c r="Q104" s="21"/>
       <c r="R104" s="21"/>
       <c r="S104" s="21"/>
       <c r="T104" s="21"/>
-      <c r="U104" s="19"/>
-    </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U104" s="21"/>
+      <c r="V104" s="19"/>
+    </row>
+    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A105" s="23"/>
       <c r="B105" s="18"/>
       <c r="C105" s="22"/>
@@ -3215,15 +3346,16 @@
       <c r="L105" s="21"/>
       <c r="M105" s="21"/>
       <c r="N105" s="21"/>
-      <c r="O105" s="22"/>
-      <c r="P105" s="21"/>
+      <c r="O105" s="21"/>
+      <c r="P105" s="22"/>
       <c r="Q105" s="21"/>
       <c r="R105" s="21"/>
       <c r="S105" s="21"/>
       <c r="T105" s="21"/>
-      <c r="U105" s="19"/>
-    </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U105" s="21"/>
+      <c r="V105" s="19"/>
+    </row>
+    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A106" s="23"/>
       <c r="B106" s="18"/>
       <c r="C106" s="22"/>
@@ -3238,15 +3370,16 @@
       <c r="L106" s="21"/>
       <c r="M106" s="21"/>
       <c r="N106" s="21"/>
-      <c r="O106" s="22"/>
-      <c r="P106" s="21"/>
+      <c r="O106" s="21"/>
+      <c r="P106" s="22"/>
       <c r="Q106" s="21"/>
       <c r="R106" s="21"/>
       <c r="S106" s="21"/>
       <c r="T106" s="21"/>
-      <c r="U106" s="19"/>
-    </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U106" s="21"/>
+      <c r="V106" s="19"/>
+    </row>
+    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A107" s="23"/>
       <c r="B107" s="18"/>
       <c r="C107" s="22"/>
@@ -3261,15 +3394,16 @@
       <c r="L107" s="21"/>
       <c r="M107" s="21"/>
       <c r="N107" s="21"/>
-      <c r="O107" s="22"/>
-      <c r="P107" s="21"/>
+      <c r="O107" s="21"/>
+      <c r="P107" s="22"/>
       <c r="Q107" s="21"/>
       <c r="R107" s="21"/>
       <c r="S107" s="21"/>
       <c r="T107" s="21"/>
-      <c r="U107" s="19"/>
-    </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U107" s="21"/>
+      <c r="V107" s="19"/>
+    </row>
+    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A108" s="23"/>
       <c r="B108" s="18"/>
       <c r="C108" s="22"/>
@@ -3284,15 +3418,16 @@
       <c r="L108" s="21"/>
       <c r="M108" s="21"/>
       <c r="N108" s="21"/>
-      <c r="O108" s="22"/>
-      <c r="P108" s="21"/>
+      <c r="O108" s="21"/>
+      <c r="P108" s="22"/>
       <c r="Q108" s="21"/>
       <c r="R108" s="21"/>
       <c r="S108" s="21"/>
       <c r="T108" s="21"/>
-      <c r="U108" s="19"/>
-    </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U108" s="21"/>
+      <c r="V108" s="19"/>
+    </row>
+    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A109" s="23"/>
       <c r="B109" s="18"/>
       <c r="C109" s="22"/>
@@ -3307,15 +3442,16 @@
       <c r="L109" s="21"/>
       <c r="M109" s="21"/>
       <c r="N109" s="21"/>
-      <c r="O109" s="22"/>
-      <c r="P109" s="21"/>
+      <c r="O109" s="21"/>
+      <c r="P109" s="22"/>
       <c r="Q109" s="21"/>
       <c r="R109" s="21"/>
       <c r="S109" s="21"/>
       <c r="T109" s="21"/>
-      <c r="U109" s="19"/>
-    </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U109" s="21"/>
+      <c r="V109" s="19"/>
+    </row>
+    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A110" s="23"/>
       <c r="B110" s="18"/>
       <c r="C110" s="22"/>
@@ -3330,19 +3466,21 @@
       <c r="L110" s="21"/>
       <c r="M110" s="21"/>
       <c r="N110" s="21"/>
-      <c r="O110" s="22"/>
-      <c r="P110" s="21"/>
+      <c r="O110" s="21"/>
+      <c r="P110" s="22"/>
       <c r="Q110" s="21"/>
       <c r="R110" s="21"/>
       <c r="S110" s="21"/>
       <c r="T110" s="21"/>
-      <c r="U110" s="19"/>
+      <c r="U110" s="21"/>
+      <c r="V110" s="19"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B3:B65391">
     <cfRule type="duplicateValues" dxfId="1" priority="8" stopIfTrue="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
+  <conditionalFormatting sqref="B2 G2 L2 Q2 V2">
     <cfRule type="duplicateValues" dxfId="0" priority="9" stopIfTrue="1"/>
   </conditionalFormatting>
   <pageMargins left="0.1" right="0.1" top="0" bottom="0.75" header="0.25" footer="0.3"/>

</xml_diff>